<commit_message>
modifing some names in sheets & modifing comments sheet
</commit_message>
<xml_diff>
--- a/Audit/Audit Sheet.xlsx
+++ b/Audit/Audit Sheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FD937C-7FF2-4C93-B490-CC363ECACE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Comment</t>
   </si>
@@ -41,12 +40,30 @@
   </si>
   <si>
     <t>Internet Banking System</t>
+  </si>
+  <si>
+    <t>Commented By</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Comment Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Close Date</t>
+  </si>
+  <si>
+    <t>comment_01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,7 +105,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -171,13 +188,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -187,6 +226,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -468,122 +509,220 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="71.21875" customWidth="1"/>
+    <col min="1" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="71.21875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>